<commit_message>
profile, balance, forgot pin otp
</commit_message>
<xml_diff>
--- a/src/test/java/testCases/otp/otpTestData.xlsx
+++ b/src/test/java/testCases/otp/otpTestData.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kevinwinarko/eclipse-workspace/DanaPulsaAutomationTest/src/test/java/testCases/otp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5863975A-6427-634A-80A2-8147F19F9FE7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28EA6126-DAB5-E443-A39D-88A68E9C7C0B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16020" activeTab="1" xr2:uid="{0BFCFD56-4938-304E-8F8D-A74A800CA122}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16020" xr2:uid="{0BFCFD56-4938-304E-8F8D-A74A800CA122}"/>
   </bookViews>
   <sheets>
-    <sheet name="ForgotPinOtp" sheetId="2" r:id="rId1"/>
+    <sheet name="ForgotPinOtp" sheetId="6" r:id="rId1"/>
     <sheet name="VerifyOtp" sheetId="4" r:id="rId2"/>
     <sheet name="GetOtp" sheetId="5" r:id="rId3"/>
   </sheets>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="9">
   <si>
     <t>id</t>
   </si>
@@ -68,18 +68,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -124,22 +116,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -150,9 +132,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -464,73 +446,47 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A09F2C92-1070-F549-ABD8-21E67EECDFEF}">
-  <dimension ref="A1:C12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14E323A5-E48C-9940-9E0A-08CF82D80C7C}">
+  <dimension ref="A1:A7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="26.5" customWidth="1"/>
-    <col min="2" max="2" width="21.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="7">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
+        <v>-155</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>9999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="3"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="7">
-        <v>-1</v>
-      </c>
-      <c r="B3" s="2"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="7">
-        <v>9999</v>
-      </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="1"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="8" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="8" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="5"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="5"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="5"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="6"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="6"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="5"/>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" s="3"/>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>181</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -541,103 +497,103 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2122BD67-CB71-784B-8957-5A1161ED6BBF}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="10">
+      <c r="A2" s="5">
+        <v>155</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="5">
+        <v>-155</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="5">
+        <v>9999</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B5" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="10">
-        <v>-1</v>
-      </c>
-      <c r="B3" s="10" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="10">
-        <v>9999</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="10" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="5">
+        <v>155</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="5">
+        <v>155</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="5">
+        <v>155</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="5">
+        <v>155</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="5">
+        <v>155</v>
+      </c>
+      <c r="B11" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="10">
-        <v>1</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="10">
-        <v>1</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="10">
-        <v>1</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="10">
-        <v>1</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="10">
-        <v>1</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>2</v>
-      </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="10"/>
-      <c r="B12" s="10"/>
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -646,42 +602,45 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3911761-BEE0-844E-B9F5-774E5EB83953}">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A6"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" s="7">
+      <c r="A2" s="2">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
+        <v>-155</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>9999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" s="7">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" s="7">
-        <v>9999</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" s="8" t="s">
-        <v>1</v>
-      </c>
-    </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" s="8" t="s">
-        <v>2</v>
+      <c r="A6" s="3"/>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" s="6">
+        <v>181</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update get otp api
</commit_message>
<xml_diff>
--- a/src/test/java/testCases/otp/otpTestData.xlsx
+++ b/src/test/java/testCases/otp/otpTestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kevinwinarko/eclipse-workspace/DanaPulsaAutomationTest/src/test/java/testCases/otp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28EA6126-DAB5-E443-A39D-88A68E9C7C0B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39B6B7EF-C414-0C4F-BDA3-732FF5FD74C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16020" xr2:uid="{0BFCFD56-4938-304E-8F8D-A74A800CA122}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16020" activeTab="2" xr2:uid="{0BFCFD56-4938-304E-8F8D-A74A800CA122}"/>
   </bookViews>
   <sheets>
     <sheet name="ForgotPinOtp" sheetId="6" r:id="rId1"/>
@@ -449,7 +449,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14E323A5-E48C-9940-9E0A-08CF82D80C7C}">
   <dimension ref="A1:A7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
@@ -602,10 +602,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3911761-BEE0-844E-B9F5-774E5EB83953}">
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -636,11 +636,8 @@
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" s="3"/>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" s="6">
-        <v>181</v>
+      <c r="A6" s="6">
+        <v>182</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update verify otp update history in progress
</commit_message>
<xml_diff>
--- a/src/test/java/testCases/otp/otpTestData.xlsx
+++ b/src/test/java/testCases/otp/otpTestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kevinwinarko/eclipse-workspace/DanaPulsaAutomationTest/src/test/java/testCases/otp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39B6B7EF-C414-0C4F-BDA3-732FF5FD74C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F51A34AE-D0F8-9144-9E75-275C627337E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16020" activeTab="2" xr2:uid="{0BFCFD56-4938-304E-8F8D-A74A800CA122}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16020" activeTab="1" xr2:uid="{0BFCFD56-4938-304E-8F8D-A74A800CA122}"/>
   </bookViews>
   <sheets>
     <sheet name="ForgotPinOtp" sheetId="6" r:id="rId1"/>
@@ -35,15 +35,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="8">
   <si>
     <t>id</t>
   </si>
   <si>
     <t>a</t>
-  </si>
-  <si>
-    <t>null</t>
   </si>
   <si>
     <t>code</t>
@@ -497,8 +494,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2122BD67-CB71-784B-8957-5A1161ED6BBF}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -508,7 +505,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -516,7 +513,7 @@
         <v>155</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -524,7 +521,7 @@
         <v>-155</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -532,7 +529,7 @@
         <v>9999</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -540,15 +537,13 @@
         <v>1</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
-        <v>2</v>
-      </c>
+      <c r="A6" s="5"/>
       <c r="B6" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -556,7 +551,7 @@
         <v>155</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -564,7 +559,7 @@
         <v>155</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -572,7 +567,7 @@
         <v>155</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -580,20 +575,22 @@
         <v>155</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="5">
         <v>155</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>2</v>
-      </c>
+      <c r="B11" s="5"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
+      <c r="A12" s="5">
+        <v>155</v>
+      </c>
+      <c r="B12" s="5">
+        <v>1234</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -604,8 +601,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3911761-BEE0-844E-B9F5-774E5EB83953}">
   <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>